<commit_message>
Atualiza dados em 28-12-2017
</commit_message>
<xml_diff>
--- a/reports/metadados.xlsx
+++ b/reports/metadados.xlsx
@@ -393,7 +393,7 @@
         </is>
       </c>
       <c r="B2" s="2">
-        <v>43096.27557086806</v>
+        <v>43097.26338454861</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -411,7 +411,7 @@
         </is>
       </c>
       <c r="B3" s="2">
-        <v>43096.26354832176</v>
+        <v>43097.27128064814</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -429,7 +429,7 @@
         </is>
       </c>
       <c r="B4" s="2">
-        <v>43096.26338003473</v>
+        <v>43097.27089083333</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B5" s="2">
-        <v>43096.30358568287</v>
+        <v>43097.30682739583</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>

</xml_diff>